<commit_message>
changed sizes of images
</commit_message>
<xml_diff>
--- a/data/material/404seiten.xlsx
+++ b/data/material/404seiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\21_404\PROJECT\404-nature-not-found\data\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD90ABC8-A44E-40E0-B3B2-037DEC2BB4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4132533-B5C4-433B-9A5C-905E5F03BA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>paint_original</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>\404material\1_marvin_anabel\original.jpg</t>
-  </si>
-  <si>
-    <t>\404material\1_marvin_anabel\00076-3903618619.png</t>
   </si>
   <si>
     <t>text_ai</t>
@@ -182,16 +179,10 @@
     <t>\404material\9_georg1\anlage.jpg</t>
   </si>
   <si>
-    <t>\404material\9_georg1\00033-1351177780.png</t>
-  </si>
-  <si>
     <t>Dieses Bild habe ich in der Nähe des Emscherbruch aufgenommen. Es ist  ein typischer Erlenbruch, wie man ihn noch häufig hier sieht. Meist sind diese an alten Flussarmen, die die Zeit überdauert haben. Das Wasser  hat sich hier gehalten und dieses Gebiet wird von Erlen dominiert, die diese große Feuchtigkeit lieben. Im Vordergrund sieht man die  frischen Triebe der gelben Wasserlilien. Das finde ich sehr reizvoll.  Sie korrespondieren gut mit dem von oben einfallenden Licht.</t>
   </si>
   <si>
     <t>\404material\10_georg2\moor.jpg</t>
-  </si>
-  <si>
-    <t>\404material\10_georg2\00023-3040446449.png</t>
   </si>
   <si>
     <t>Maur´ícioMM</t>
@@ -211,12 +202,6 @@
 </t>
   </si>
   <si>
-    <t>\404material\12_rainer\00002-372827910.png</t>
-  </si>
-  <si>
-    <t>\404material\12_rainer\00001-3817646381.png</t>
-  </si>
-  <si>
     <t>name_ai</t>
   </si>
   <si>
@@ -266,13 +251,7 @@
     <t>Ich schlendere entlang des Emscherufers und bemerke einen seltsamen Zaun, der mitten im Fluss steht. Neugierig gehe ich näher heran und entdecke, dass dieser Zaun mit hunderten von kunstvoll bemalten Schlössern geschmückt ist. Jedes Schloss trägt den Namen eines Liebespaares und ist mit den Initialen und dem Datum ihrer Verbundenheit graviert. Es ist ein romantischer Anblick, der mich lächeln lässt. Inmitten der rauen Industrielandschaft und der Renaturierungsmaßnahmen hat dieser Zaun ein Stück Liebe und Hoffnung eingefangen. Ich nehme mir einen Moment, um die Geschichten hinter den Schlössern zu erahnen und fühle mich von der Magie der Emscher verzaubert.</t>
   </si>
   <si>
-    <t>\404material\16_chatgpt\00099-4139572241.png</t>
-  </si>
-  <si>
     <t>In der weiten Landschaft der Emscher Region erblühte mein Leben, als ich gerade drei Jahre alt war. Die Natur war mein Rückzugsort, ein Ort voller Wunder und Schönheit. Doch an einem traurigen Tag verlor ich meine Mutter, als drei majestätische Eichen durch einen Sturm entwurzelt wurden. Ihr Verlust traf mich wie ein herzzerreißender Schlag. Die Natur, die einst meine Zuflucht war, fühlte sich nun düster und unheimlich an. Doch im Laufe der Zeit entdeckte ich in den leuchtenden Blüten der Emscherwiesen und den sanften Klängen des fließenden Wassers einen Hauch von Trost. Die Natur heilte meine Wunden, und ich fand Frieden in der Verbindung zwischen Mensch und Umwelt in der Emscher Region.</t>
-  </si>
-  <si>
-    <t>\404material\17_chatgpt\00131-1792453834.png</t>
   </si>
   <si>
     <t>Ich stehe am Ufer der Emscher und betrachte das ruhige Wasser, als plötzlich etwas Metallisches angespült wird. Neugierig bücke ich mich und greife nach dem Gegenstand. Es ist eine Zylinderkopfdichtung! Verwundert frage ich mich, wie eine Autoteilkomponente hierher gelangen konnte. Inmitten der Renaturierungsmaßnahmen und der räumlichen Enge zwischen Natur und Stadt scheint diese Entdeckung fehl am Platz. Doch dann erinnere ich mich an die industrielle Vergangenheit der Region, in der Autowerke und Fabriken einst den Alltag prägten. Die Zylinderkopfdichtung wird zu einem Symbol für den Wandel und die Transformation der Emscher. Es ist ein Hinweis darauf, dass sich die Zeiten geändert haben und sich die Region nun einem neuen Kapitel zuwendet - von der Industrie zur Erholung und Erneuerung. Mit einem Lächeln lasse ich die Zylinderkopfdichtung ins Wasser gleiten und hoffe, dass sie als Erinnerung an vergangene Zeiten und die Zukunft der Emscher dienen wird.</t>
@@ -285,14 +264,38 @@
 </t>
   </si>
   <si>
-    <t>\404material\19_chatgpt\00102-4139572241.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Die Sonne steht hoch am Himmel, als ich durch den renovierten Emscherpark schlendere. Plötzlich vernimmt mein Ohr einen vertrauten Klang – das Zwitschern von Papageien. Ich halte inne und schaue genauer hin. Tatsächlich sitzen bunte Papageien auf den Ästen der Bäume und lassen ihre farbenfrohen Federn im Wind schimmern. Ein Lächeln breitet sich auf meinem Gesicht aus. Wer hätte gedacht, dass sich diese exotischen Vögel hier niederlassen würden? In der Emscher Region gibt es immer wieder Überraschungen zu entdecken.
 </t>
   </si>
   <si>
     <t>\404material\20_chatgpt\00047-2332438302.png</t>
+  </si>
+  <si>
+    <t>\404material\1_marvin_anabel\00076-3903618619.jpg</t>
+  </si>
+  <si>
+    <t>\404material\6_bärbel\00008-1158096131.jpg</t>
+  </si>
+  <si>
+    <t>\404material\9_georg1\00033-1351177780.jpg</t>
+  </si>
+  <si>
+    <t>\404material\10_georg2\00023-3040446449.jpg</t>
+  </si>
+  <si>
+    <t>\404material\12_rainer\00002-372827910.jpg</t>
+  </si>
+  <si>
+    <t>\404material\12_rainer\00001-3817646381.jpg</t>
+  </si>
+  <si>
+    <t>\404material\16_chatgpt\00099-4139572241.jpg</t>
+  </si>
+  <si>
+    <t>\404material\17_chatgpt\00131-1792453834.jpg</t>
+  </si>
+  <si>
+    <t>\404material\19_chatgpt\00102-4139572241.jpg</t>
   </si>
 </sst>
 </file>
@@ -335,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -343,17 +346,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -641,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,520 +655,520 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="390" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" ht="285" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" ht="390" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="195" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" ht="390" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="270" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
+      <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" ht="270" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" ht="270" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" ht="285" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" ht="390" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" ht="300" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" ht="225" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>

</xml_diff>

<commit_message>
added last drawings so that every 404 side has at leats one drawing
</commit_message>
<xml_diff>
--- a/data/material/404seiten.xlsx
+++ b/data/material/404seiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\21_404\PROJECT\404-nature-not-found\data\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4132533-B5C4-433B-9A5C-905E5F03BA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA5AACC-D1C7-4334-8E79-5AFDD5ECA9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>paint_original</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>\404material\19_chatgpt\00102-4139572241.jpg</t>
+  </si>
+  <si>
+    <t>\404material\11_mauricio\00001-4277853085.jpg</t>
+  </si>
+  <si>
+    <t>\404material\11_mauricio\00002-4277853086.jpg</t>
+  </si>
+  <si>
+    <t>\404material\12_rainer\00003-2366520323.jpg</t>
   </si>
 </sst>
 </file>
@@ -637,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +789,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -956,8 +965,12 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
@@ -978,7 +991,9 @@
         <v>84</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>

</xml_diff>

<commit_message>
fixed problem with image name in xls
</commit_message>
<xml_diff>
--- a/data/material/404seiten.xlsx
+++ b/data/material/404seiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\21_404\PROJECT\404-nature-not-found\data\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA5AACC-D1C7-4334-8E79-5AFDD5ECA9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD178EA-6C09-4626-877C-84DEE8D91473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>\404material\6_bärbel\dog (Small).jpg</t>
   </si>
   <si>
-    <t>\404material\6_bärbel\00008-1158096131.png</t>
-  </si>
-  <si>
     <t>\404material\6_bärbel\00001-1150433406.png</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>\404material\12_rainer\00003-2366520323.jpg</t>
+  </si>
+  <si>
+    <t>\404material\6_bärbel\00008-2736945635.png</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -733,7 +733,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -849,32 +849,32 @@
         <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -885,18 +885,18 @@
     </row>
     <row r="10" spans="1:12" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -907,92 +907,92 @@
     </row>
     <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1000,10 +1000,10 @@
     <row r="15" spans="1:12" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
@@ -1012,7 +1012,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1020,10 +1020,10 @@
     <row r="16" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1032,7 +1032,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1040,10 +1040,10 @@
     <row r="17" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1052,7 +1052,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1060,10 +1060,10 @@
     <row r="18" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1072,7 +1072,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1080,10 +1080,10 @@
     <row r="19" spans="1:12" ht="285" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1092,7 +1092,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1100,10 +1100,10 @@
     <row r="20" spans="1:12" ht="390" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1112,7 +1112,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1120,10 +1120,10 @@
     <row r="21" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1132,7 +1132,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1140,10 +1140,10 @@
     <row r="22" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1152,7 +1152,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>

</xml_diff>